<commit_message>
changed coment on healthy people
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\Tracy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4171F97-EEBB-4261-BDEE-BAE6437E9EC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CDA7C0-0FC0-4432-8E27-A9BAF2052745}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="160">
   <si>
     <t>index</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>MET-min/week</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> new variable could be created coded =0 for all participants</t>
   </si>
 </sst>
 </file>
@@ -923,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1510,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>51</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
KARMEN-3 PREV_HYP: Comment section has been updated by giving reason why participants were giving 0 catergory. PREV_CVD: Wrong comment has been changed to CVD instead of diabetes.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77F4513-F410-4240-A77E-C29BE02A7F8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBBEC3-F6B6-44E9-ACC3-F1EA142225EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="161">
   <si>
     <t>index</t>
   </si>
@@ -499,7 +499,10 @@
     <t>MET-min/week</t>
   </si>
   <si>
-    <t xml:space="preserve"> new variable could be created coded =0 for all participants</t>
+    <t>due to inclusion criteria, all participants were healthy at time of reruitment without a history of hypertension; new variable could be created coded =0 for all participants</t>
+  </si>
+  <si>
+    <t>due to inclusion criteria, all participants were healthy at time of reruitment without a history of CVD; new variable could be created coded =0 for all participants</t>
   </si>
 </sst>
 </file>
@@ -926,25 +929,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -979,7 +982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -1207,7 +1210,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1234,7 +1237,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1315,7 +1318,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>41</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>43</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>45</v>
       </c>
@@ -1454,7 +1457,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>49</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="135" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>51</v>
       </c>
@@ -1539,7 +1542,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>53</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>135</v>
@@ -1568,7 +1571,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>57</v>
       </c>
@@ -1626,7 +1629,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>59</v>
       </c>
@@ -1655,7 +1658,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>61</v>
       </c>
@@ -1684,7 +1687,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>63</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>65</v>
       </c>
@@ -1742,7 +1745,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>67</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>71</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>75</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>77</v>
       </c>
@@ -1916,7 +1919,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" ht="120" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -1945,7 +1948,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>81</v>
       </c>
@@ -1974,7 +1977,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>83</v>
       </c>
@@ -2003,7 +2006,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>85</v>
       </c>
@@ -2032,7 +2035,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>87</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>89</v>
       </c>
@@ -2090,7 +2093,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>91</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>93</v>
       </c>
@@ -2148,7 +2151,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>97</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>99</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>101</v>
       </c>
@@ -2264,7 +2267,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>103</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>105</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>107</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>109</v>
       </c>
@@ -2380,7 +2383,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>111</v>
       </c>
@@ -2409,7 +2412,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>113</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>115</v>
       </c>
@@ -2467,7 +2470,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>117</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>119</v>
       </c>
@@ -2525,7 +2528,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -2554,7 +2557,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>124</v>
       </c>
@@ -2583,7 +2586,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>126</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>128</v>
       </c>
@@ -2641,7 +2644,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>130</v>
       </c>
@@ -2670,7 +2673,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
KARMEN-3 MED_STAT:Wrong comment has been updated to fit the statement Standard meta data sheet provided MED_NSAID:Wrong comment has been updated to fit the statement Standard meta data sheet provided
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CBBEC3-F6B6-44E9-ACC3-F1EA142225EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884380C-5EE0-43CC-89F2-403295680127}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="162">
   <si>
     <t>index</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t>due to inclusion criteria, all participants were healthy at time of reruitment without a history of CVD; new variable could be created coded =0 for all participants</t>
+  </si>
+  <si>
+    <t>due to inclusion criteria, no medication for all included participants; new variable could be created coded =0 for all participants</t>
   </si>
 </sst>
 </file>
@@ -929,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,7 +1893,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>77</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>135</v>
@@ -1919,7 +1922,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="105" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>135</v>

</xml_diff>

<commit_message>
KARMEN-3 SMOKING STATUS: all participants have been grouped in category 4 because status is unknown
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9884380C-5EE0-43CC-89F2-403295680127}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588FBD70-E9B1-46BF-AAC8-46235504A5A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="164">
   <si>
     <t>index</t>
   </si>
@@ -506,6 +506,12 @@
   </si>
   <si>
     <t>due to inclusion criteria, no medication for all included participants; new variable could be created coded =0 for all participants</t>
+  </si>
+  <si>
+    <t>all included participants are current non-smokers; no information available on former smoking</t>
+  </si>
+  <si>
+    <t>partial</t>
   </si>
 </sst>
 </file>
@@ -932,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1132,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1136,23 +1142,23 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>140</v>
+      <c r="F7" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>141</v>
+        <v>151</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
KARMEN-3 SMOKING STATUS: Changes has been made to my comment to fit what Franzi has wriiten for her DPE and Harmo Status details changed to proximate.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588FBD70-E9B1-46BF-AAC8-46235504A5A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8116516-8446-4347-8F4F-861EA9010352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,10 +508,10 @@
     <t>due to inclusion criteria, no medication for all included participants; new variable could be created coded =0 for all participants</t>
   </si>
   <si>
-    <t>all included participants are current non-smokers; no information available on former smoking</t>
-  </si>
-  <si>
     <t>partial</t>
+  </si>
+  <si>
+    <t>non-smokers as inclusion criterion, but we cannot be sure, if they are real never smokers or former smokers</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -598,6 +598,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,7 +940,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1133,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1151,14 +1152,14 @@
       <c r="H7" s="3">
         <v>4</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="K7" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
KARMEN-3: TOT_PA_QX: harmon. status changed to complete and details changed to compatible. Algorithm changed Contraceptive:harmo. status to immopsible and details to incompatible Menopause: Recoded to 1:0 and 2:1
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_proc_elem/DPE_KARMEN_TRACY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\analyst\Tracy\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8116516-8446-4347-8F4F-861EA9010352}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222D6C8B-8883-4DCB-B3F9-C82AA69C6E87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,9 +454,6 @@
     <t>operation</t>
   </si>
   <si>
-    <t>(IPAQ_MET_Total*60)/7</t>
-  </si>
-  <si>
     <t>compatible</t>
   </si>
   <si>
@@ -469,9 +466,6 @@
     <t>recode</t>
   </si>
   <si>
-    <t>recode(0=1;1=2;)</t>
-  </si>
-  <si>
     <t>__BLANK__</t>
   </si>
   <si>
@@ -481,9 +475,6 @@
     <t>no HRT for all included women due to inclusion criteria, new variable could be created coded such as HRT=0</t>
   </si>
   <si>
-    <t>all included women did not take contraceptives due to inclusion criteria, new variable could be created coding all participants =0</t>
-  </si>
-  <si>
     <t>due to inclusion criteria, all participants were healthy at time of reruitment without a history of diabetes; new variable could be created coded =0 for all participants</t>
   </si>
   <si>
@@ -512,6 +503,15 @@
   </si>
   <si>
     <t>non-smokers as inclusion criterion, but we cannot be sure, if they are real never smokers or former smokers</t>
+  </si>
+  <si>
+    <t>(IPAQ_MET_Total/60)/7</t>
+  </si>
+  <si>
+    <t>incompatible</t>
+  </si>
+  <si>
+    <t>recode(1=0;2=1;)</t>
   </si>
 </sst>
 </file>
@@ -939,25 +939,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -992,7 +992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>134</v>
@@ -1021,7 +1021,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>16</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>19</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -1121,19 +1121,19 @@
         <v>143</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1144,25 +1144,25 @@
         <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H7" s="3">
         <v>4</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>29</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>31</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>33</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -1366,23 +1366,23 @@
         <v>13</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>41</v>
       </c>
@@ -1393,25 +1393,25 @@
         <v>13</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H16" s="3">
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="90" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>43</v>
       </c>
@@ -1421,26 +1421,24 @@
       <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>150</v>
+      <c r="F17" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="4" t="s">
+        <v>140</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>45</v>
       </c>
@@ -1467,7 +1465,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>47</v>
       </c>
@@ -1494,7 +1492,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>49</v>
       </c>
@@ -1505,25 +1503,25 @@
         <v>13</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H20" s="3">
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="135" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>51</v>
       </c>
@@ -1534,25 +1532,25 @@
         <v>13</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H21" s="3">
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>53</v>
       </c>
@@ -1563,25 +1561,25 @@
         <v>13</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H22" s="3">
         <v>0</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="120" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>55</v>
       </c>
@@ -1592,25 +1590,25 @@
         <v>13</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H23" s="3">
         <v>0</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>57</v>
       </c>
@@ -1624,7 +1622,7 @@
         <v>140</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>140</v>
@@ -1639,7 +1637,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>59</v>
       </c>
@@ -1653,7 +1651,7 @@
         <v>140</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>140</v>
@@ -1668,7 +1666,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>61</v>
       </c>
@@ -1682,7 +1680,7 @@
         <v>140</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>140</v>
@@ -1697,7 +1695,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>63</v>
       </c>
@@ -1711,7 +1709,7 @@
         <v>140</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>140</v>
@@ -1726,7 +1724,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>65</v>
       </c>
@@ -1740,7 +1738,7 @@
         <v>140</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>140</v>
@@ -1755,7 +1753,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>67</v>
       </c>
@@ -1769,7 +1767,7 @@
         <v>140</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>140</v>
@@ -1778,13 +1776,13 @@
         <v>141</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>69</v>
       </c>
@@ -1798,7 +1796,7 @@
         <v>140</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>140</v>
@@ -1813,7 +1811,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>71</v>
       </c>
@@ -1827,7 +1825,7 @@
         <v>140</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>140</v>
@@ -1842,7 +1840,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>73</v>
       </c>
@@ -1856,7 +1854,7 @@
         <v>140</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>140</v>
@@ -1871,7 +1869,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>75</v>
       </c>
@@ -1885,7 +1883,7 @@
         <v>140</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>140</v>
@@ -1900,7 +1898,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>77</v>
       </c>
@@ -1911,25 +1909,25 @@
         <v>13</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H34" s="3">
         <v>0</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" ht="105" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -1940,25 +1938,25 @@
         <v>13</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H35" s="3">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>135</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>81</v>
       </c>
@@ -1987,7 +1985,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>83</v>
       </c>
@@ -2016,7 +2014,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>85</v>
       </c>
@@ -2045,7 +2043,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>87</v>
       </c>
@@ -2074,7 +2072,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>89</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>91</v>
       </c>
@@ -2132,7 +2130,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>93</v>
       </c>
@@ -2161,7 +2159,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>95</v>
       </c>
@@ -2190,7 +2188,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>97</v>
       </c>
@@ -2219,7 +2217,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>99</v>
       </c>
@@ -2248,7 +2246,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>101</v>
       </c>
@@ -2277,7 +2275,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>103</v>
       </c>
@@ -2306,7 +2304,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>105</v>
       </c>
@@ -2335,7 +2333,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>107</v>
       </c>
@@ -2364,7 +2362,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>109</v>
       </c>
@@ -2393,7 +2391,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>111</v>
       </c>
@@ -2422,7 +2420,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>113</v>
       </c>
@@ -2451,7 +2449,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>115</v>
       </c>
@@ -2480,7 +2478,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>117</v>
       </c>
@@ -2509,7 +2507,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>119</v>
       </c>
@@ -2538,7 +2536,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>122</v>
       </c>
@@ -2567,7 +2565,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>124</v>
       </c>
@@ -2596,7 +2594,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>126</v>
       </c>
@@ -2625,7 +2623,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>128</v>
       </c>
@@ -2654,7 +2652,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>130</v>
       </c>
@@ -2683,7 +2681,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>132</v>
       </c>

</xml_diff>